<commit_message>
working up updating goals. removed RC goal. changed ICO to CON (connection to place). updated HAB and CP.
</commit_message>
<xml_diff>
--- a/prep/R/rc_NOAA_soc_survey.xlsx
+++ b/prep/R/rc_NOAA_soc_survey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36460" yWindow="-1500" windowWidth="29940" windowHeight="16200" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-36460" yWindow="-1500" windowWidth="29940" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,6 +290,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -299,15 +306,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="65">
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1891,35 +1891,35 @@
         <v>12</v>
       </c>
       <c r="E19" s="2">
-        <f>E15/SUM(E$12:E$15)</f>
+        <f t="shared" ref="E19:L19" si="15">E15/SUM(E$12:E$15)</f>
         <v>0.35218093699515346</v>
       </c>
       <c r="F19" s="2">
-        <f>F15/SUM(F$12:F$15)</f>
+        <f t="shared" si="15"/>
         <v>0.17235772357723578</v>
       </c>
       <c r="G19" s="2">
-        <f>G15/SUM(G$12:G$15)</f>
+        <f t="shared" si="15"/>
         <v>9.3851132686084138E-2</v>
       </c>
       <c r="H19" s="2">
-        <f>H15/SUM(H$12:H$15)</f>
+        <f t="shared" si="15"/>
         <v>8.2658022690437608E-2</v>
       </c>
       <c r="I19" s="2">
-        <f>I15/SUM(I$12:I$15)</f>
+        <f t="shared" si="15"/>
         <v>0.22977346278317151</v>
       </c>
       <c r="J19" s="2">
-        <f>J15/SUM(J$12:J$15)</f>
+        <f t="shared" si="15"/>
         <v>6.8071312803889783E-2</v>
       </c>
       <c r="K19" s="2">
-        <f>K15/SUM(K$12:K$15)</f>
+        <f t="shared" si="15"/>
         <v>0.13570274636510501</v>
       </c>
       <c r="L19" s="2">
-        <f>L15/SUM(L$12:L$15)</f>
+        <f t="shared" si="15"/>
         <v>6.9579288025889974E-2</v>
       </c>
       <c r="O19" s="2"/>
@@ -1944,31 +1944,31 @@
         <v>0.82714054927302105</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" ref="F20:L20" si="15">1-F16</f>
+        <f t="shared" ref="F20:L20" si="16">1-F16</f>
         <v>0.60813008130081303</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.3381877022653722</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.54457050243111826</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.81229773462783172</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.33387358184764993</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.36833602584814218</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.30744336569579289</v>
       </c>
       <c r="O20" s="2"/>
@@ -2643,31 +2643,31 @@
         <v>0.14354066985645933</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" ref="F29:L29" si="16">F25/SUM(F$25:F$28)</f>
+        <f t="shared" ref="F29:L29" si="17">F25/SUM(F$25:F$28)</f>
         <v>0.40284360189573459</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.62411347517730498</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.40380047505938244</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.12826603325415678</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.60952380952380958</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.50591016548463352</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.57311320754716977</v>
       </c>
       <c r="O29" s="2"/>
@@ -2694,35 +2694,35 @@
         <v>10</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" ref="E30:E31" si="17">E26/SUM(E$25:E$28)</f>
+        <f t="shared" ref="E30:E31" si="18">E26/SUM(E$25:E$28)</f>
         <v>0.23444976076555024</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" ref="F30:L30" si="18">F26/SUM(F$25:F$28)</f>
+        <f t="shared" ref="F30:L30" si="19">F26/SUM(F$25:F$28)</f>
         <v>0.32701421800947866</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.18912529550827423</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.42280285035629456</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.34679334916864607</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.26904761904761904</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.20803782505910165</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.30424528301886794</v>
       </c>
       <c r="O30" s="2"/>
@@ -2750,35 +2750,35 @@
         <v>11</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.14832535885167464</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" ref="F31:L31" si="19">F27/SUM(F$25:F$28)</f>
+        <f t="shared" ref="F31:L31" si="20">F27/SUM(F$25:F$28)</f>
         <v>8.7677725118483416E-2</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.4373522458628844E-2</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.7885985748218529E-2</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.18764845605700711</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4.0476190476190478E-2</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.2009456264775412E-2</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.6603773584905662E-2</v>
       </c>
       <c r="O31" s="2"/>
@@ -2810,31 +2810,31 @@
         <v>0.47368421052631576</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" ref="F32:L32" si="20">F28/SUM(F$25:F$28)</f>
+        <f t="shared" ref="F32:L32" si="21">F28/SUM(F$25:F$28)</f>
         <v>0.18246445497630331</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.13238770685579196</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>8.5510688836104506E-2</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.33729216152019004</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>8.0952380952380956E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.23404255319148937</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.6037735849056603E-2</v>
       </c>
       <c r="O32" s="2"/>
@@ -2859,31 +2859,31 @@
         <v>0.8564593301435407</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" ref="F33:L33" si="21">1-F29</f>
+        <f t="shared" ref="F33:L33" si="22">1-F29</f>
         <v>0.59715639810426535</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.37588652482269502</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.59619952494061756</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.87173396674584325</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.39047619047619042</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.49408983451536648</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.42688679245283023</v>
       </c>
     </row>
@@ -3545,43 +3545,43 @@
         <v>9</v>
       </c>
       <c r="E42">
-        <f>SUM(E21,E34,E38)</f>
+        <f t="shared" ref="E42:N42" si="23">SUM(E21,E34,E38)</f>
         <v>94</v>
       </c>
       <c r="F42">
-        <f>SUM(F21,F34,F38)</f>
+        <f t="shared" si="23"/>
         <v>213</v>
       </c>
       <c r="G42">
-        <f>SUM(G21,G34,G38)</f>
+        <f t="shared" si="23"/>
         <v>339</v>
       </c>
       <c r="H42">
-        <f>SUM(H21,H34,H38)</f>
+        <f t="shared" si="23"/>
         <v>263</v>
       </c>
       <c r="I42">
-        <f>SUM(I21,I34,I38)</f>
+        <f t="shared" si="23"/>
         <v>106</v>
       </c>
       <c r="J42">
-        <f>SUM(J21,J34,J38)</f>
+        <f t="shared" si="23"/>
         <v>328</v>
       </c>
       <c r="K42">
-        <f>SUM(K21,K34,K38)</f>
+        <f t="shared" si="23"/>
         <v>287</v>
       </c>
       <c r="L42">
-        <f>SUM(L21,L34,L38)</f>
+        <f t="shared" si="23"/>
         <v>353</v>
       </c>
       <c r="M42">
-        <f>SUM(M21,M34,M38)</f>
+        <f t="shared" si="23"/>
         <v>308</v>
       </c>
       <c r="N42">
-        <f>SUM(N21,N34,N38)</f>
+        <f t="shared" si="23"/>
         <v>359</v>
       </c>
       <c r="O42" s="2">
@@ -3635,43 +3635,43 @@
         <v>10</v>
       </c>
       <c r="E43">
-        <f>SUM(E22,E35,E39)</f>
+        <f t="shared" ref="E43:N43" si="24">SUM(E22,E35,E39)</f>
         <v>120</v>
       </c>
       <c r="F43">
-        <f>SUM(F22,F35,F39)</f>
+        <f t="shared" si="24"/>
         <v>165</v>
       </c>
       <c r="G43">
-        <f>SUM(G22,G35,G39)</f>
+        <f t="shared" si="24"/>
         <v>100</v>
       </c>
       <c r="H43">
-        <f>SUM(H22,H35,H39)</f>
+        <f t="shared" si="24"/>
         <v>191</v>
       </c>
       <c r="I43">
-        <f>SUM(I22,I35,I39)</f>
+        <f t="shared" si="24"/>
         <v>183</v>
       </c>
       <c r="J43">
-        <f>SUM(J22,J35,J39)</f>
+        <f t="shared" si="24"/>
         <v>145</v>
       </c>
       <c r="K43">
-        <f>SUM(K22,K35,K39)</f>
+        <f t="shared" si="24"/>
         <v>97</v>
       </c>
       <c r="L43">
-        <f>SUM(L22,L35,L39)</f>
+        <f t="shared" si="24"/>
         <v>116</v>
       </c>
       <c r="M43">
-        <f>SUM(M22,M35,M39)</f>
+        <f t="shared" si="24"/>
         <v>124</v>
       </c>
       <c r="N43">
-        <f>SUM(N22,N35,N39)</f>
+        <f t="shared" si="24"/>
         <v>110</v>
       </c>
       <c r="O43" s="2">
@@ -3726,43 +3726,43 @@
         <v>11</v>
       </c>
       <c r="E44">
-        <f>SUM(E23,E36,E40)</f>
+        <f t="shared" ref="E44:N44" si="25">SUM(E23,E36,E40)</f>
         <v>71</v>
       </c>
       <c r="F44">
-        <f>SUM(F23,F36,F40)</f>
+        <f t="shared" si="25"/>
         <v>49</v>
       </c>
       <c r="G44">
-        <f>SUM(G23,G36,G40)</f>
+        <f t="shared" si="25"/>
         <v>32</v>
       </c>
       <c r="H44">
-        <f>SUM(H23,H36,H40)</f>
+        <f t="shared" si="25"/>
         <v>45</v>
       </c>
       <c r="I44">
-        <f>SUM(I23,I36,I40)</f>
+        <f t="shared" si="25"/>
         <v>96</v>
       </c>
       <c r="J44">
-        <f>SUM(J23,J36,J40)</f>
+        <f t="shared" si="25"/>
         <v>27</v>
       </c>
       <c r="K44">
-        <f>SUM(K23,K36,K40)</f>
+        <f t="shared" si="25"/>
         <v>46</v>
       </c>
       <c r="L44">
-        <f>SUM(L23,L36,L40)</f>
+        <f t="shared" si="25"/>
         <v>28</v>
       </c>
       <c r="M44">
-        <f>SUM(M23,M36,M40)</f>
+        <f t="shared" si="25"/>
         <v>38</v>
       </c>
       <c r="N44">
-        <f>SUM(N23,N36,N40)</f>
+        <f t="shared" si="25"/>
         <v>35</v>
       </c>
       <c r="O44" s="2">
@@ -3817,43 +3817,43 @@
         <v>12</v>
       </c>
       <c r="E45">
-        <f>SUM(E24,E37,E41)</f>
+        <f t="shared" ref="E45:N45" si="26">SUM(E24,E37,E41)</f>
         <v>248</v>
       </c>
       <c r="F45">
-        <f>SUM(F24,F37,F41)</f>
+        <f t="shared" si="26"/>
         <v>107</v>
       </c>
       <c r="G45">
-        <f>SUM(G24,G37,G41)</f>
+        <f t="shared" si="26"/>
         <v>69</v>
       </c>
       <c r="H45">
-        <f>SUM(H24,H37,H41)</f>
+        <f t="shared" si="26"/>
         <v>38</v>
       </c>
       <c r="I45">
-        <f>SUM(I24,I37,I41)</f>
+        <f t="shared" si="26"/>
         <v>154</v>
       </c>
       <c r="J45">
-        <f>SUM(J24,J37,J41)</f>
+        <f t="shared" si="26"/>
         <v>37</v>
       </c>
       <c r="K45">
-        <f>SUM(K24,K37,K41)</f>
+        <f t="shared" si="26"/>
         <v>112</v>
       </c>
       <c r="L45">
-        <f>SUM(L24,L37,L41)</f>
+        <f t="shared" si="26"/>
         <v>44</v>
       </c>
       <c r="M45">
-        <f>SUM(M24,M37,M41)</f>
+        <f t="shared" si="26"/>
         <v>71</v>
       </c>
       <c r="N45">
-        <f>SUM(N24,N37,N41)</f>
+        <f t="shared" si="26"/>
         <v>34</v>
       </c>
       <c r="O45" s="2">
@@ -3978,43 +3978,43 @@
         <v>9</v>
       </c>
       <c r="E47" s="2">
-        <f>E42/SUM(E$42:E$45)</f>
+        <f t="shared" ref="E47:N47" si="27">E42/SUM(E$42:E$45)</f>
         <v>0.17636022514071295</v>
       </c>
       <c r="F47" s="2">
-        <f>F42/SUM(F$42:F$45)</f>
+        <f t="shared" si="27"/>
         <v>0.398876404494382</v>
       </c>
       <c r="G47" s="2">
-        <f>G42/SUM(G$42:G$45)</f>
+        <f t="shared" si="27"/>
         <v>0.62777777777777777</v>
       </c>
       <c r="H47" s="2">
-        <f>H42/SUM(H$42:H$45)</f>
+        <f t="shared" si="27"/>
         <v>0.48975791433891991</v>
       </c>
       <c r="I47" s="2">
-        <f>I42/SUM(I$42:I$45)</f>
+        <f t="shared" si="27"/>
         <v>0.19666048237476808</v>
       </c>
       <c r="J47" s="2">
-        <f>J42/SUM(J$42:J$45)</f>
+        <f t="shared" si="27"/>
         <v>0.61080074487895719</v>
       </c>
       <c r="K47" s="2">
-        <f>K42/SUM(K$42:K$45)</f>
+        <f t="shared" si="27"/>
         <v>0.52952029520295207</v>
       </c>
       <c r="L47" s="2">
-        <f>L42/SUM(L$42:L$45)</f>
+        <f t="shared" si="27"/>
         <v>0.65249537892791132</v>
       </c>
       <c r="M47" s="2">
-        <f>M42/SUM(M$42:M$45)</f>
+        <f t="shared" si="27"/>
         <v>0.56931608133086875</v>
       </c>
       <c r="N47" s="2">
-        <f>N42/SUM(N$42:N$45)</f>
+        <f t="shared" si="27"/>
         <v>0.66728624535315983</v>
       </c>
     </row>
@@ -4032,43 +4032,43 @@
         <v>10</v>
       </c>
       <c r="E48" s="2">
-        <f>E43/SUM(E$42:E$45)</f>
+        <f t="shared" ref="E48:N48" si="28">E43/SUM(E$42:E$45)</f>
         <v>0.22514071294559099</v>
       </c>
       <c r="F48" s="2">
-        <f>F43/SUM(F$42:F$45)</f>
+        <f t="shared" si="28"/>
         <v>0.3089887640449438</v>
       </c>
       <c r="G48" s="2">
-        <f>G43/SUM(G$42:G$45)</f>
+        <f t="shared" si="28"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="H48" s="2">
-        <f>H43/SUM(H$42:H$45)</f>
+        <f t="shared" si="28"/>
         <v>0.35567970204841715</v>
       </c>
       <c r="I48" s="2">
-        <f>I43/SUM(I$42:I$45)</f>
+        <f t="shared" si="28"/>
         <v>0.33951762523191092</v>
       </c>
       <c r="J48" s="2">
-        <f>J43/SUM(J$42:J$45)</f>
+        <f t="shared" si="28"/>
         <v>0.27001862197392923</v>
       </c>
       <c r="K48" s="2">
-        <f>K43/SUM(K$42:K$45)</f>
+        <f t="shared" si="28"/>
         <v>0.17896678966789667</v>
       </c>
       <c r="L48" s="2">
-        <f>L43/SUM(L$42:L$45)</f>
+        <f t="shared" si="28"/>
         <v>0.2144177449168207</v>
       </c>
       <c r="M48" s="2">
-        <f>M43/SUM(M$42:M$45)</f>
+        <f t="shared" si="28"/>
         <v>0.22920517560073936</v>
       </c>
       <c r="N48" s="2">
-        <f>N43/SUM(N$42:N$45)</f>
+        <f t="shared" si="28"/>
         <v>0.20446096654275092</v>
       </c>
     </row>
@@ -4087,43 +4087,43 @@
         <v>11</v>
       </c>
       <c r="E49" s="2">
-        <f>E44/SUM(E$42:E$45)</f>
+        <f t="shared" ref="E49:N49" si="29">E44/SUM(E$42:E$45)</f>
         <v>0.13320825515947468</v>
       </c>
       <c r="F49" s="2">
-        <f>F44/SUM(F$42:F$45)</f>
+        <f t="shared" si="29"/>
         <v>9.1760299625468167E-2</v>
       </c>
       <c r="G49" s="2">
-        <f>G44/SUM(G$42:G$45)</f>
+        <f t="shared" si="29"/>
         <v>5.9259259259259262E-2</v>
       </c>
       <c r="H49" s="2">
-        <f>H44/SUM(H$42:H$45)</f>
+        <f t="shared" si="29"/>
         <v>8.3798882681564241E-2</v>
       </c>
       <c r="I49" s="2">
-        <f>I44/SUM(I$42:I$45)</f>
+        <f t="shared" si="29"/>
         <v>0.17810760667903525</v>
       </c>
       <c r="J49" s="2">
-        <f>J44/SUM(J$42:J$45)</f>
+        <f t="shared" si="29"/>
         <v>5.027932960893855E-2</v>
       </c>
       <c r="K49" s="2">
-        <f>K44/SUM(K$42:K$45)</f>
+        <f t="shared" si="29"/>
         <v>8.4870848708487087E-2</v>
       </c>
       <c r="L49" s="2">
-        <f>L44/SUM(L$42:L$45)</f>
+        <f t="shared" si="29"/>
         <v>5.1756007393715345E-2</v>
       </c>
       <c r="M49" s="2">
-        <f>M44/SUM(M$42:M$45)</f>
+        <f t="shared" si="29"/>
         <v>7.0240295748613679E-2</v>
       </c>
       <c r="N49" s="2">
-        <f>N44/SUM(N$42:N$45)</f>
+        <f t="shared" si="29"/>
         <v>6.5055762081784388E-2</v>
       </c>
     </row>
@@ -4142,43 +4142,43 @@
         <v>12</v>
       </c>
       <c r="E50" s="2">
-        <f>E45/SUM(E$42:E$45)</f>
+        <f t="shared" ref="E50:N50" si="30">E45/SUM(E$42:E$45)</f>
         <v>0.46529080675422141</v>
       </c>
       <c r="F50" s="2">
-        <f>F45/SUM(F$42:F$45)</f>
+        <f t="shared" si="30"/>
         <v>0.20037453183520598</v>
       </c>
       <c r="G50" s="2">
-        <f>G45/SUM(G$42:G$45)</f>
+        <f t="shared" si="30"/>
         <v>0.12777777777777777</v>
       </c>
       <c r="H50" s="2">
-        <f>H45/SUM(H$42:H$45)</f>
+        <f t="shared" si="30"/>
         <v>7.0763500931098691E-2</v>
       </c>
       <c r="I50" s="2">
-        <f>I45/SUM(I$42:I$45)</f>
+        <f t="shared" si="30"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="J50" s="2">
-        <f>J45/SUM(J$42:J$45)</f>
+        <f t="shared" si="30"/>
         <v>6.8901303538175043E-2</v>
       </c>
       <c r="K50" s="2">
-        <f>K45/SUM(K$42:K$45)</f>
+        <f t="shared" si="30"/>
         <v>0.20664206642066421</v>
       </c>
       <c r="L50" s="2">
-        <f>L45/SUM(L$42:L$45)</f>
+        <f t="shared" si="30"/>
         <v>8.1330868761552683E-2</v>
       </c>
       <c r="M50" s="2">
-        <f>M45/SUM(M$42:M$45)</f>
+        <f t="shared" si="30"/>
         <v>0.13123844731977818</v>
       </c>
       <c r="N50" s="2">
-        <f>N45/SUM(N$42:N$45)</f>
+        <f t="shared" si="30"/>
         <v>6.3197026022304828E-2</v>
       </c>
     </row>
@@ -4194,39 +4194,39 @@
         <v>0.82363977485928708</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" ref="F51:N51" si="22">1-F47</f>
+        <f t="shared" ref="F51:N51" si="31">1-F47</f>
         <v>0.601123595505618</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.37222222222222223</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.51024208566108009</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.80333951762523192</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.38919925512104281</v>
       </c>
       <c r="K51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.47047970479704793</v>
       </c>
       <c r="L51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.34750462107208868</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.43068391866913125</v>
       </c>
       <c r="N51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>0.33271375464684017</v>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -4992,7 +4992,7 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="6">
@@ -5038,7 +5038,7 @@
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="13"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="6">
         <v>2</v>
       </c>
@@ -5082,7 +5082,7 @@
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="13"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="6">
         <v>3</v>
       </c>
@@ -5126,7 +5126,7 @@
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="13"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="6">
         <v>4</v>
       </c>
@@ -5170,7 +5170,7 @@
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="6">
@@ -5216,7 +5216,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="13"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="6">
         <v>2</v>
       </c>
@@ -5260,7 +5260,7 @@
       </c>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="13"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="6">
         <v>3</v>
       </c>
@@ -5304,7 +5304,7 @@
       </c>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="13"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="6">
         <v>4</v>
       </c>
@@ -5348,7 +5348,7 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="6">
@@ -5394,7 +5394,7 @@
       </c>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="13"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="6">
         <v>2</v>
       </c>
@@ -5438,7 +5438,7 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="13"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="6">
         <v>3</v>
       </c>
@@ -5482,7 +5482,7 @@
       </c>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="13"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="6">
         <v>4</v>
       </c>
@@ -5526,141 +5526,141 @@
       </c>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="15">
-        <v>1</v>
-      </c>
-      <c r="C35" s="15">
+      <c r="B35" s="12">
+        <v>1</v>
+      </c>
+      <c r="C35" s="12">
         <v>0</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="13">
         <f t="shared" ref="E35:L35" si="12">E14*100</f>
         <v>14.354066985645932</v>
       </c>
-      <c r="F35" s="16">
+      <c r="F35" s="13">
         <f t="shared" si="12"/>
         <v>40.284360189573462</v>
       </c>
-      <c r="G35" s="16">
+      <c r="G35" s="13">
         <f t="shared" si="12"/>
         <v>62.411347517730498</v>
       </c>
-      <c r="H35" s="16">
+      <c r="H35" s="13">
         <f t="shared" si="12"/>
         <v>40.380047505938244</v>
       </c>
-      <c r="I35" s="16">
+      <c r="I35" s="13">
         <f t="shared" si="12"/>
         <v>12.826603325415679</v>
       </c>
-      <c r="J35" s="16">
+      <c r="J35" s="13">
         <f t="shared" si="12"/>
         <v>60.952380952380956</v>
       </c>
-      <c r="K35" s="16">
+      <c r="K35" s="13">
         <f t="shared" si="12"/>
         <v>50.591016548463351</v>
       </c>
-      <c r="L35" s="16">
+      <c r="L35" s="13">
         <f t="shared" si="12"/>
         <v>57.311320754716974</v>
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15">
+      <c r="A36" s="17"/>
+      <c r="B36" s="12">
         <v>2</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="12">
         <v>12</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="13">
         <f t="shared" ref="E36:L36" si="13">E15*100</f>
         <v>23.444976076555022</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="13">
         <f t="shared" si="13"/>
         <v>32.70142180094787</v>
       </c>
-      <c r="G36" s="16">
+      <c r="G36" s="13">
         <f t="shared" si="13"/>
         <v>18.912529550827422</v>
       </c>
-      <c r="H36" s="16">
+      <c r="H36" s="13">
         <f t="shared" si="13"/>
         <v>42.280285035629454</v>
       </c>
-      <c r="I36" s="16">
+      <c r="I36" s="13">
         <f t="shared" si="13"/>
         <v>34.679334916864605</v>
       </c>
-      <c r="J36" s="16">
+      <c r="J36" s="13">
         <f t="shared" si="13"/>
         <v>26.904761904761905</v>
       </c>
-      <c r="K36" s="16">
+      <c r="K36" s="13">
         <f t="shared" si="13"/>
         <v>20.803782505910164</v>
       </c>
-      <c r="L36" s="16">
+      <c r="L36" s="13">
         <f t="shared" si="13"/>
         <v>30.424528301886795</v>
       </c>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15">
+      <c r="A37" s="17"/>
+      <c r="B37" s="12">
         <v>3</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="12">
         <v>30</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="13">
         <f t="shared" ref="E37:L37" si="14">E16*100</f>
         <v>14.832535885167463</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="13">
         <f t="shared" si="14"/>
         <v>8.7677725118483423</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="13">
         <f t="shared" si="14"/>
         <v>5.4373522458628845</v>
       </c>
-      <c r="H37" s="16">
+      <c r="H37" s="13">
         <f t="shared" si="14"/>
         <v>8.7885985748218527</v>
       </c>
-      <c r="I37" s="16">
+      <c r="I37" s="13">
         <f t="shared" si="14"/>
         <v>18.76484560570071</v>
       </c>
-      <c r="J37" s="16">
+      <c r="J37" s="13">
         <f t="shared" si="14"/>
         <v>4.0476190476190474</v>
       </c>
-      <c r="K37" s="16">
+      <c r="K37" s="13">
         <f t="shared" si="14"/>
         <v>5.2009456264775409</v>
       </c>
-      <c r="L37" s="16">
+      <c r="L37" s="13">
         <f t="shared" si="14"/>
         <v>5.6603773584905666</v>
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="17"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="8">
         <v>4</v>
       </c>
@@ -5670,35 +5670,35 @@
       <c r="D38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="14">
         <f t="shared" ref="E38:L38" si="15">E17*100</f>
         <v>47.368421052631575</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F38" s="14">
         <f t="shared" si="15"/>
         <v>18.246445497630333</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="14">
         <f t="shared" si="15"/>
         <v>13.238770685579196</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H38" s="14">
         <f t="shared" si="15"/>
         <v>8.5510688836104514</v>
       </c>
-      <c r="I38" s="18">
+      <c r="I38" s="14">
         <f t="shared" si="15"/>
         <v>33.729216152019006</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="14">
         <f t="shared" si="15"/>
         <v>8.0952380952380949</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="14">
         <f t="shared" si="15"/>
         <v>23.404255319148938</v>
       </c>
-      <c r="L38" s="18">
+      <c r="L38" s="14">
         <f t="shared" si="15"/>
         <v>6.6037735849056602</v>
       </c>

</xml_diff>